<commit_message>
update file and fix ImportClass
</commit_message>
<xml_diff>
--- a/import/danhsachlop.xlsx
+++ b/import/danhsachlop.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\nckh_ng\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nckh\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127F789E-4381-47EA-B3DD-9A6E50A81FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A620040-7690-4E54-A941-5538580397BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8F6D045-6FE1-44B9-9070-279A78C0176E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8F6D045-6FE1-44B9-9070-279A78C0176E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -34,29 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
-  <si>
-    <t>Lớp CNTT 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>CNTT101</t>
   </si>
   <si>
-    <t>HK1</t>
-  </si>
-  <si>
     <t>2025-2026</t>
   </si>
   <si>
-    <t>Lớp CNTT 2</t>
-  </si>
-  <si>
     <t>CNTT102</t>
   </si>
   <si>
-    <t>HK2</t>
-  </si>
-  <si>
     <t>tên_lớp</t>
   </si>
   <si>
@@ -78,27 +66,12 @@
     <t>gv001</t>
   </si>
   <si>
-    <t>Thiết kế Đồ Họa</t>
-  </si>
-  <si>
     <t>DHTT202</t>
   </si>
   <si>
     <t>gv002</t>
   </si>
   <si>
-    <t>Thiết kế Họa Tiết</t>
-  </si>
-  <si>
-    <t>Thiết kế Giao Diện</t>
-  </si>
-  <si>
-    <t>Thiết kế Hệ Thống</t>
-  </si>
-  <si>
-    <t>Thiết kế Vật liệu</t>
-  </si>
-  <si>
     <t>DHTT203</t>
   </si>
   <si>
@@ -109,6 +82,27 @@
   </si>
   <si>
     <t>DHTT206</t>
+  </si>
+  <si>
+    <t>mon_hoc</t>
+  </si>
+  <si>
+    <t>B202A</t>
+  </si>
+  <si>
+    <t>B203A</t>
+  </si>
+  <si>
+    <t>B202B</t>
+  </si>
+  <si>
+    <t>B303A</t>
+  </si>
+  <si>
+    <t>B302A</t>
+  </si>
+  <si>
+    <t>B402A</t>
   </si>
 </sst>
 </file>
@@ -119,7 +113,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -127,13 +121,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -188,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -197,11 +191,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -217,9 +210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -257,7 +250,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -363,7 +356,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -505,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,271 +506,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69C4282-326E-4D37-918D-A5D8A7CB62FC}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="1" max="1" width="20.8984375" customWidth="1"/>
+    <col min="2" max="2" width="15.296875" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
+    <col min="4" max="5" width="14.19921875" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>